<commit_message>
Alteração 2 código automação email
</commit_message>
<xml_diff>
--- a/projeto automação e-mail/base email.xlsx
+++ b/projeto automação e-mail/base email.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>condomínio</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>clientesdiasdeofertas+nota@gmail.com</t>
+  </si>
+  <si>
+    <t>canopus</t>
   </si>
 </sst>
 </file>
@@ -344,6 +347,17 @@
         <v>9</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>